<commit_message>
corrections, all sections - 21.06.2022
</commit_message>
<xml_diff>
--- a/ExpLog_FieldNotes.xlsx
+++ b/ExpLog_FieldNotes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A890204-B33A-F843-9825-3C8A3B50D53E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C25D1F2-AFE3-9B4C-AF07-214EABDC389E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment Log" sheetId="1" r:id="rId1"/>
@@ -1676,56 +1676,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2017,10 +2017,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A25" sqref="A25"/>
-      <selection pane="topRight" activeCell="O18" sqref="O18"/>
+      <selection pane="topRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2300,312 +2300,312 @@
       <c r="AF6" s="62"/>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="114" t="s">
+      <c r="C7" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="114" t="s">
+      <c r="D7" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="114" t="s">
+      <c r="E7" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="114" t="s">
+      <c r="G7" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="114" t="s">
+      <c r="H7" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="114" t="s">
+      <c r="I7" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="114" t="s">
+      <c r="J7" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="114" t="s">
+      <c r="K7" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="L7" s="114" t="s">
+      <c r="L7" s="122" t="s">
         <v>118</v>
       </c>
-      <c r="M7" s="114" t="s">
+      <c r="M7" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="N7" s="114" t="s">
+      <c r="N7" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="O7" s="112" t="s">
+      <c r="O7" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="P7" s="112" t="s">
+      <c r="P7" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="Q7" s="112" t="s">
+      <c r="Q7" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="R7" s="112" t="s">
+      <c r="R7" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="S7" s="112" t="s">
+      <c r="S7" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="T7" s="112" t="s">
+      <c r="T7" s="125" t="s">
         <v>118</v>
       </c>
-      <c r="U7" s="112" t="s">
+      <c r="U7" s="125" t="s">
         <v>244</v>
       </c>
-      <c r="V7" s="112" t="s">
+      <c r="V7" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="W7" s="112" t="s">
+      <c r="W7" s="125" t="s">
         <v>256</v>
       </c>
-      <c r="X7" s="112" t="s">
+      <c r="X7" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="Y7" s="112" t="s">
+      <c r="Y7" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="Z7" s="112" t="s">
+      <c r="Z7" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="AA7" s="113"/>
-      <c r="AB7" s="111"/>
-      <c r="AC7" s="111"/>
-      <c r="AD7" s="111"/>
-      <c r="AE7" s="111"/>
-      <c r="AF7" s="111"/>
+      <c r="AA7" s="126"/>
+      <c r="AB7" s="127"/>
+      <c r="AC7" s="127"/>
+      <c r="AD7" s="127"/>
+      <c r="AE7" s="127"/>
+      <c r="AF7" s="127"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" s="115"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="114"/>
-      <c r="K8" s="114"/>
-      <c r="L8" s="114"/>
-      <c r="M8" s="114"/>
-      <c r="N8" s="114"/>
-      <c r="O8" s="112"/>
-      <c r="P8" s="112"/>
-      <c r="Q8" s="112"/>
-      <c r="R8" s="112"/>
-      <c r="S8" s="112"/>
-      <c r="T8" s="112"/>
-      <c r="U8" s="112"/>
-      <c r="V8" s="112"/>
-      <c r="W8" s="112"/>
-      <c r="X8" s="112"/>
-      <c r="Y8" s="112"/>
-      <c r="Z8" s="112"/>
-      <c r="AA8" s="113"/>
-      <c r="AB8" s="111"/>
-      <c r="AC8" s="111"/>
-      <c r="AD8" s="111"/>
-      <c r="AE8" s="111"/>
-      <c r="AF8" s="111"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="124"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="122"/>
+      <c r="K8" s="122"/>
+      <c r="L8" s="122"/>
+      <c r="M8" s="122"/>
+      <c r="N8" s="122"/>
+      <c r="O8" s="125"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="125"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
+      <c r="T8" s="125"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="125"/>
+      <c r="W8" s="125"/>
+      <c r="X8" s="125"/>
+      <c r="Y8" s="125"/>
+      <c r="Z8" s="125"/>
+      <c r="AA8" s="126"/>
+      <c r="AB8" s="127"/>
+      <c r="AC8" s="127"/>
+      <c r="AD8" s="127"/>
+      <c r="AE8" s="127"/>
+      <c r="AF8" s="127"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
-      <c r="B9" s="116"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="114"/>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="114"/>
-      <c r="O9" s="112"/>
-      <c r="P9" s="112"/>
-      <c r="Q9" s="112"/>
-      <c r="R9" s="112"/>
-      <c r="S9" s="112"/>
-      <c r="T9" s="112"/>
-      <c r="U9" s="112"/>
-      <c r="V9" s="112"/>
-      <c r="W9" s="112"/>
-      <c r="X9" s="112"/>
-      <c r="Y9" s="112"/>
-      <c r="Z9" s="112"/>
-      <c r="AA9" s="113"/>
-      <c r="AB9" s="111"/>
-      <c r="AC9" s="111"/>
-      <c r="AD9" s="111"/>
-      <c r="AE9" s="111"/>
-      <c r="AF9" s="111"/>
+      <c r="A9" s="123"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="122"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="122"/>
+      <c r="O9" s="125"/>
+      <c r="P9" s="125"/>
+      <c r="Q9" s="125"/>
+      <c r="R9" s="125"/>
+      <c r="S9" s="125"/>
+      <c r="T9" s="125"/>
+      <c r="U9" s="125"/>
+      <c r="V9" s="125"/>
+      <c r="W9" s="125"/>
+      <c r="X9" s="125"/>
+      <c r="Y9" s="125"/>
+      <c r="Z9" s="125"/>
+      <c r="AA9" s="126"/>
+      <c r="AB9" s="127"/>
+      <c r="AC9" s="127"/>
+      <c r="AD9" s="127"/>
+      <c r="AE9" s="127"/>
+      <c r="AF9" s="127"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="114" t="s">
+      <c r="C10" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="114" t="s">
+      <c r="D10" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="114" t="s">
+      <c r="E10" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="114" t="s">
+      <c r="F10" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="114" t="s">
+      <c r="G10" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="114" t="s">
+      <c r="H10" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="114" t="s">
+      <c r="I10" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="114" t="s">
+      <c r="J10" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="114" t="s">
+      <c r="K10" s="122" t="s">
         <v>118</v>
       </c>
-      <c r="L10" s="114" t="s">
+      <c r="L10" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="M10" s="114" t="s">
+      <c r="M10" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="N10" s="114" t="s">
+      <c r="N10" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="112" t="s">
+      <c r="O10" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="P10" s="112" t="s">
+      <c r="P10" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="Q10" s="112" t="s">
+      <c r="Q10" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="R10" s="112" t="s">
+      <c r="R10" s="125" t="s">
         <v>118</v>
       </c>
-      <c r="S10" s="112" t="s">
+      <c r="S10" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="T10" s="112" t="s">
+      <c r="T10" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="U10" s="112" t="s">
+      <c r="U10" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="V10" s="112" t="s">
+      <c r="V10" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="W10" s="112" t="s">
+      <c r="W10" s="125" t="s">
         <v>260</v>
       </c>
-      <c r="X10" s="112" t="s">
+      <c r="X10" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="Y10" s="112" t="s">
+      <c r="Y10" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="Z10" s="112" t="s">
+      <c r="Z10" s="125" t="s">
         <v>73</v>
       </c>
-      <c r="AA10" s="113"/>
-      <c r="AB10" s="111"/>
-      <c r="AC10" s="111"/>
-      <c r="AD10" s="111"/>
-      <c r="AE10" s="111"/>
-      <c r="AF10" s="111"/>
+      <c r="AA10" s="126"/>
+      <c r="AB10" s="127"/>
+      <c r="AC10" s="127"/>
+      <c r="AD10" s="127"/>
+      <c r="AE10" s="127"/>
+      <c r="AF10" s="127"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" s="115"/>
-      <c r="B11" s="116"/>
-      <c r="C11" s="114"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="114"/>
-      <c r="K11" s="114"/>
-      <c r="L11" s="114"/>
-      <c r="M11" s="114"/>
-      <c r="N11" s="114"/>
-      <c r="O11" s="112"/>
-      <c r="P11" s="112"/>
-      <c r="Q11" s="112"/>
-      <c r="R11" s="112"/>
-      <c r="S11" s="112"/>
-      <c r="T11" s="112"/>
-      <c r="U11" s="112"/>
-      <c r="V11" s="112"/>
-      <c r="W11" s="112"/>
-      <c r="X11" s="112"/>
-      <c r="Y11" s="112"/>
-      <c r="Z11" s="112"/>
-      <c r="AA11" s="113"/>
-      <c r="AB11" s="111"/>
-      <c r="AC11" s="111"/>
-      <c r="AD11" s="111"/>
-      <c r="AE11" s="111"/>
-      <c r="AF11" s="111"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="122"/>
+      <c r="M11" s="122"/>
+      <c r="N11" s="122"/>
+      <c r="O11" s="125"/>
+      <c r="P11" s="125"/>
+      <c r="Q11" s="125"/>
+      <c r="R11" s="125"/>
+      <c r="S11" s="125"/>
+      <c r="T11" s="125"/>
+      <c r="U11" s="125"/>
+      <c r="V11" s="125"/>
+      <c r="W11" s="125"/>
+      <c r="X11" s="125"/>
+      <c r="Y11" s="125"/>
+      <c r="Z11" s="125"/>
+      <c r="AA11" s="126"/>
+      <c r="AB11" s="127"/>
+      <c r="AC11" s="127"/>
+      <c r="AD11" s="127"/>
+      <c r="AE11" s="127"/>
+      <c r="AF11" s="127"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A12" s="115"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="114"/>
-      <c r="K12" s="114"/>
-      <c r="L12" s="114"/>
-      <c r="M12" s="114"/>
-      <c r="N12" s="114"/>
-      <c r="O12" s="112"/>
-      <c r="P12" s="112"/>
-      <c r="Q12" s="112"/>
-      <c r="R12" s="112"/>
-      <c r="S12" s="112"/>
-      <c r="T12" s="112"/>
-      <c r="U12" s="112"/>
-      <c r="V12" s="112"/>
-      <c r="W12" s="112"/>
-      <c r="X12" s="112"/>
-      <c r="Y12" s="112"/>
-      <c r="Z12" s="112"/>
-      <c r="AA12" s="113"/>
-      <c r="AB12" s="111"/>
-      <c r="AC12" s="111"/>
-      <c r="AD12" s="111"/>
-      <c r="AE12" s="111"/>
-      <c r="AF12" s="111"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="122"/>
+      <c r="M12" s="122"/>
+      <c r="N12" s="122"/>
+      <c r="O12" s="125"/>
+      <c r="P12" s="125"/>
+      <c r="Q12" s="125"/>
+      <c r="R12" s="125"/>
+      <c r="S12" s="125"/>
+      <c r="T12" s="125"/>
+      <c r="U12" s="125"/>
+      <c r="V12" s="125"/>
+      <c r="W12" s="125"/>
+      <c r="X12" s="125"/>
+      <c r="Y12" s="125"/>
+      <c r="Z12" s="125"/>
+      <c r="AA12" s="126"/>
+      <c r="AB12" s="127"/>
+      <c r="AC12" s="127"/>
+      <c r="AD12" s="127"/>
+      <c r="AE12" s="127"/>
+      <c r="AF12" s="127"/>
     </row>
     <row r="13" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="87" t="s">
@@ -2694,7 +2694,7 @@
       <c r="AF13" s="63"/>
     </row>
     <row r="14" spans="1:32" s="38" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="122" t="s">
+      <c r="A14" s="119" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="90"/>
@@ -2736,7 +2736,7 @@
       <c r="AF14" s="64"/>
     </row>
     <row r="15" spans="1:32" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="123"/>
+      <c r="A15" s="120"/>
       <c r="B15" s="92"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2776,7 +2776,7 @@
       <c r="AF15" s="64"/>
     </row>
     <row r="16" spans="1:32" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="123"/>
+      <c r="A16" s="120"/>
       <c r="B16" s="92"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -2816,7 +2816,7 @@
       <c r="AF16" s="64"/>
     </row>
     <row r="17" spans="1:32" ht="75" x14ac:dyDescent="0.2">
-      <c r="A17" s="124"/>
+      <c r="A17" s="121"/>
       <c r="B17" s="92"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -2856,7 +2856,7 @@
       <c r="AF17" s="64"/>
     </row>
     <row r="18" spans="1:32" ht="60" x14ac:dyDescent="0.2">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="119" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="92"/>
@@ -2898,7 +2898,7 @@
       <c r="AF18" s="64"/>
     </row>
     <row r="19" spans="1:32" ht="60" x14ac:dyDescent="0.2">
-      <c r="A19" s="123"/>
+      <c r="A19" s="120"/>
       <c r="B19" s="92"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2936,7 +2936,7 @@
       <c r="AF19" s="64"/>
     </row>
     <row r="20" spans="1:32" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="123"/>
+      <c r="A20" s="120"/>
       <c r="B20" s="92"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2974,7 +2974,7 @@
       <c r="AF20" s="64"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A21" s="124"/>
+      <c r="A21" s="121"/>
       <c r="B21" s="92"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -3008,7 +3008,7 @@
       <c r="AF21" s="64"/>
     </row>
     <row r="22" spans="1:32" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="122" t="s">
+      <c r="A22" s="119" t="s">
         <v>80</v>
       </c>
       <c r="B22" s="92"/>
@@ -3050,7 +3050,7 @@
       <c r="AF22" s="64"/>
     </row>
     <row r="23" spans="1:32" ht="105" x14ac:dyDescent="0.2">
-      <c r="A23" s="123"/>
+      <c r="A23" s="120"/>
       <c r="B23" s="92"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -3088,7 +3088,7 @@
       <c r="AF23" s="64"/>
     </row>
     <row r="24" spans="1:32" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="123"/>
+      <c r="A24" s="120"/>
       <c r="B24" s="92"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -3126,7 +3126,7 @@
       <c r="AF24" s="64"/>
     </row>
     <row r="25" spans="1:32" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="124"/>
+      <c r="A25" s="121"/>
       <c r="B25" s="93"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -3164,7 +3164,7 @@
       <c r="AF25" s="65"/>
     </row>
     <row r="26" spans="1:32" ht="60" x14ac:dyDescent="0.2">
-      <c r="A26" s="122" t="s">
+      <c r="A26" s="119" t="s">
         <v>81</v>
       </c>
       <c r="B26" s="93"/>
@@ -3206,7 +3206,7 @@
       <c r="AF26" s="65"/>
     </row>
     <row r="27" spans="1:32" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="123"/>
+      <c r="A27" s="120"/>
       <c r="B27" s="93"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -3246,7 +3246,7 @@
       <c r="AF27" s="65"/>
     </row>
     <row r="28" spans="1:32" ht="45" x14ac:dyDescent="0.2">
-      <c r="A28" s="123"/>
+      <c r="A28" s="120"/>
       <c r="B28" s="93"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -3284,7 +3284,7 @@
       <c r="AF28" s="65"/>
     </row>
     <row r="29" spans="1:32" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="124"/>
+      <c r="A29" s="121"/>
       <c r="B29" s="94"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -3322,7 +3322,7 @@
       <c r="AF29" s="63"/>
     </row>
     <row r="30" spans="1:32" ht="135" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="120" t="s">
+      <c r="A30" s="117" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="95"/>
@@ -3364,7 +3364,7 @@
       <c r="AF30" s="63"/>
     </row>
     <row r="31" spans="1:32" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="121"/>
+      <c r="A31" s="118"/>
       <c r="B31" s="95"/>
       <c r="C31" s="36"/>
       <c r="D31" s="36"/>
@@ -3402,7 +3402,7 @@
       <c r="AF31" s="63"/>
     </row>
     <row r="32" spans="1:32" ht="105" x14ac:dyDescent="0.2">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="114" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="96" t="s">
@@ -3488,7 +3488,7 @@
       <c r="AF32" s="66"/>
     </row>
     <row r="33" spans="1:32" ht="103" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="118"/>
+      <c r="A33" s="115"/>
       <c r="B33" s="97" t="s">
         <v>20</v>
       </c>
@@ -3571,8 +3571,8 @@
       <c r="AE33" s="67"/>
       <c r="AF33" s="67"/>
     </row>
-    <row r="34" spans="1:32" ht="150" x14ac:dyDescent="0.2">
-      <c r="A34" s="118"/>
+    <row r="34" spans="1:32" ht="135" x14ac:dyDescent="0.2">
+      <c r="A34" s="115"/>
       <c r="B34" s="97" t="s">
         <v>23</v>
       </c>
@@ -3651,8 +3651,8 @@
       <c r="AE34" s="67"/>
       <c r="AF34" s="67"/>
     </row>
-    <row r="35" spans="1:32" ht="180" x14ac:dyDescent="0.2">
-      <c r="A35" s="118"/>
+    <row r="35" spans="1:32" ht="165" x14ac:dyDescent="0.2">
+      <c r="A35" s="115"/>
       <c r="B35" s="97" t="s">
         <v>24</v>
       </c>
@@ -3732,7 +3732,7 @@
       <c r="AF35" s="67"/>
     </row>
     <row r="36" spans="1:32" ht="150" x14ac:dyDescent="0.2">
-      <c r="A36" s="118"/>
+      <c r="A36" s="115"/>
       <c r="B36" s="97"/>
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
@@ -3804,7 +3804,7 @@
       <c r="AF36" s="67"/>
     </row>
     <row r="37" spans="1:32" ht="90" x14ac:dyDescent="0.2">
-      <c r="A37" s="118"/>
+      <c r="A37" s="115"/>
       <c r="B37" s="97"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
@@ -3872,7 +3872,7 @@
       <c r="AF37" s="67"/>
     </row>
     <row r="38" spans="1:32" ht="120" x14ac:dyDescent="0.2">
-      <c r="A38" s="118"/>
+      <c r="A38" s="115"/>
       <c r="B38" s="98"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -3932,7 +3932,7 @@
       <c r="AF38" s="67"/>
     </row>
     <row r="39" spans="1:32" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="118"/>
+      <c r="A39" s="115"/>
       <c r="B39" s="98"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -3982,7 +3982,7 @@
       <c r="AF39" s="67"/>
     </row>
     <row r="40" spans="1:32" ht="225" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="118"/>
+      <c r="A40" s="115"/>
       <c r="B40" s="98"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -4030,7 +4030,7 @@
       <c r="AF40" s="67"/>
     </row>
     <row r="41" spans="1:32" ht="120" x14ac:dyDescent="0.2">
-      <c r="A41" s="118"/>
+      <c r="A41" s="115"/>
       <c r="B41" s="98"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -4076,7 +4076,7 @@
       <c r="AF41" s="67"/>
     </row>
     <row r="42" spans="1:32" ht="45" x14ac:dyDescent="0.2">
-      <c r="A42" s="118"/>
+      <c r="A42" s="115"/>
       <c r="B42" s="98"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
@@ -4116,7 +4116,7 @@
       <c r="AF42" s="67"/>
     </row>
     <row r="43" spans="1:32" ht="45" x14ac:dyDescent="0.2">
-      <c r="A43" s="118"/>
+      <c r="A43" s="115"/>
       <c r="B43" s="98"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
@@ -4154,7 +4154,7 @@
       <c r="AF43" s="67"/>
     </row>
     <row r="44" spans="1:32" ht="76" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="119"/>
+      <c r="A44" s="116"/>
       <c r="B44" s="99"/>
       <c r="C44" s="100"/>
       <c r="D44" s="100"/>
@@ -4327,12 +4327,54 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A32:A44"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="AB10:AB12"/>
+    <mergeCell ref="AC10:AC12"/>
+    <mergeCell ref="AD10:AD12"/>
+    <mergeCell ref="AE10:AE12"/>
+    <mergeCell ref="AF10:AF12"/>
+    <mergeCell ref="AD7:AD9"/>
+    <mergeCell ref="AE7:AE9"/>
+    <mergeCell ref="AF7:AF9"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="P10:P12"/>
+    <mergeCell ref="Q10:Q12"/>
+    <mergeCell ref="R10:R12"/>
+    <mergeCell ref="S10:S12"/>
+    <mergeCell ref="T10:T12"/>
+    <mergeCell ref="U10:U12"/>
+    <mergeCell ref="V10:V12"/>
+    <mergeCell ref="W10:W12"/>
+    <mergeCell ref="X10:X12"/>
+    <mergeCell ref="Y10:Y12"/>
+    <mergeCell ref="Z10:Z12"/>
+    <mergeCell ref="AA10:AA12"/>
+    <mergeCell ref="Y7:Y9"/>
+    <mergeCell ref="Z7:Z9"/>
+    <mergeCell ref="AA7:AA9"/>
+    <mergeCell ref="AB7:AB9"/>
+    <mergeCell ref="AC7:AC9"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="U7:U9"/>
+    <mergeCell ref="V7:V9"/>
+    <mergeCell ref="W7:W9"/>
+    <mergeCell ref="X7:X9"/>
+    <mergeCell ref="O7:O9"/>
+    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="Q7:Q9"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="S7:S9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="M7:M9"/>
@@ -4349,54 +4391,12 @@
     <mergeCell ref="L10:L12"/>
     <mergeCell ref="M10:M12"/>
     <mergeCell ref="N10:N12"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="O7:O9"/>
-    <mergeCell ref="P7:P9"/>
-    <mergeCell ref="Q7:Q9"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="S7:S9"/>
-    <mergeCell ref="T7:T9"/>
-    <mergeCell ref="U7:U9"/>
-    <mergeCell ref="V7:V9"/>
-    <mergeCell ref="W7:W9"/>
-    <mergeCell ref="X7:X9"/>
-    <mergeCell ref="Y7:Y9"/>
-    <mergeCell ref="Z7:Z9"/>
-    <mergeCell ref="AA7:AA9"/>
-    <mergeCell ref="AB7:AB9"/>
-    <mergeCell ref="AC7:AC9"/>
-    <mergeCell ref="AD7:AD9"/>
-    <mergeCell ref="AE7:AE9"/>
-    <mergeCell ref="AF7:AF9"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="P10:P12"/>
-    <mergeCell ref="Q10:Q12"/>
-    <mergeCell ref="R10:R12"/>
-    <mergeCell ref="S10:S12"/>
-    <mergeCell ref="T10:T12"/>
-    <mergeCell ref="U10:U12"/>
-    <mergeCell ref="V10:V12"/>
-    <mergeCell ref="W10:W12"/>
-    <mergeCell ref="X10:X12"/>
-    <mergeCell ref="Y10:Y12"/>
-    <mergeCell ref="Z10:Z12"/>
-    <mergeCell ref="AA10:AA12"/>
-    <mergeCell ref="AB10:AB12"/>
-    <mergeCell ref="AC10:AC12"/>
-    <mergeCell ref="AD10:AD12"/>
-    <mergeCell ref="AE10:AE12"/>
-    <mergeCell ref="AF10:AF12"/>
+    <mergeCell ref="A32:A44"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5605,8 +5605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5F9BAE-87C6-894F-A41B-BB234234BCD4}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5614,8 +5614,9 @@
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="126" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="112" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -5628,7 +5629,7 @@
       <c r="C1" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="125" t="s">
+      <c r="D1" s="111" t="s">
         <v>327</v>
       </c>
       <c r="E1" s="13" t="s">
@@ -5647,7 +5648,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5657,7 +5658,7 @@
       <c r="C2" t="s">
         <v>289</v>
       </c>
-      <c r="D2" s="126">
+      <c r="D2" s="112">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -5669,8 +5670,11 @@
       <c r="G2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I2" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5680,7 +5684,7 @@
       <c r="C3" t="s">
         <v>290</v>
       </c>
-      <c r="D3" s="126">
+      <c r="D3" s="112">
         <v>1</v>
       </c>
       <c r="E3" t="s">
@@ -5692,8 +5696,11 @@
       <c r="G3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I3" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5703,7 +5710,7 @@
       <c r="C4" t="s">
         <v>291</v>
       </c>
-      <c r="D4" s="126">
+      <c r="D4" s="112">
         <v>1</v>
       </c>
       <c r="E4" t="s">
@@ -5715,8 +5722,11 @@
       <c r="G4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I4" s="32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5726,7 +5736,7 @@
       <c r="C5" t="s">
         <v>292</v>
       </c>
-      <c r="D5" s="126">
+      <c r="D5" s="112">
         <v>1</v>
       </c>
       <c r="E5" t="s">
@@ -5737,6 +5747,9 @@
       </c>
       <c r="G5" t="s">
         <v>32</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.2">
@@ -5749,7 +5762,7 @@
       <c r="C6" t="s">
         <v>285</v>
       </c>
-      <c r="D6" s="126">
+      <c r="D6" s="112">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -5761,9 +5774,7 @@
       <c r="G6" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="32" t="s">
-        <v>83</v>
-      </c>
+      <c r="I6" s="32"/>
       <c r="J6" s="106" t="s">
         <v>183</v>
       </c>
@@ -5778,7 +5789,7 @@
       <c r="C7" t="s">
         <v>286</v>
       </c>
-      <c r="D7" s="126">
+      <c r="D7" s="112">
         <v>2</v>
       </c>
       <c r="E7" t="s">
@@ -5790,9 +5801,7 @@
       <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="32" t="s">
-        <v>86</v>
-      </c>
+      <c r="I7" s="32"/>
       <c r="J7" s="109" t="s">
         <v>184</v>
       </c>
@@ -5809,7 +5818,7 @@
       <c r="C8" t="s">
         <v>287</v>
       </c>
-      <c r="D8" s="126">
+      <c r="D8" s="112">
         <v>2</v>
       </c>
       <c r="E8" t="s">
@@ -5821,9 +5830,7 @@
       <c r="G8" t="s">
         <v>310</v>
       </c>
-      <c r="I8" s="32" t="s">
-        <v>84</v>
-      </c>
+      <c r="I8" s="32"/>
       <c r="J8" s="109" t="s">
         <v>182</v>
       </c>
@@ -5840,7 +5847,7 @@
       <c r="C9" t="s">
         <v>288</v>
       </c>
-      <c r="D9" s="126">
+      <c r="D9" s="112">
         <v>2</v>
       </c>
       <c r="E9" t="s">
@@ -5852,9 +5859,7 @@
       <c r="G9" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="32" t="s">
-        <v>85</v>
-      </c>
+      <c r="I9" s="32"/>
       <c r="J9" s="50" t="s">
         <v>185</v>
       </c>
@@ -5869,7 +5874,7 @@
       <c r="C10" s="107" t="s">
         <v>298</v>
       </c>
-      <c r="D10" s="127" t="s">
+      <c r="D10" s="113" t="s">
         <v>328</v>
       </c>
       <c r="E10" t="s">
@@ -5898,7 +5903,7 @@
       <c r="C11" t="s">
         <v>299</v>
       </c>
-      <c r="D11" s="126">
+      <c r="D11" s="112">
         <v>1</v>
       </c>
       <c r="E11" t="s">
@@ -5927,7 +5932,7 @@
       <c r="C12" s="107" t="s">
         <v>300</v>
       </c>
-      <c r="D12" s="127" t="s">
+      <c r="D12" s="113" t="s">
         <v>328</v>
       </c>
       <c r="E12" t="s">
@@ -5956,7 +5961,7 @@
       <c r="C13" t="s">
         <v>301</v>
       </c>
-      <c r="D13" s="126">
+      <c r="D13" s="112">
         <v>1</v>
       </c>
       <c r="E13" t="s">
@@ -5985,7 +5990,7 @@
       <c r="C14" t="s">
         <v>303</v>
       </c>
-      <c r="D14" s="126">
+      <c r="D14" s="112">
         <v>2</v>
       </c>
       <c r="E14" t="s">
@@ -6014,7 +6019,7 @@
       <c r="C15" t="s">
         <v>304</v>
       </c>
-      <c r="D15" s="126">
+      <c r="D15" s="112">
         <v>2</v>
       </c>
       <c r="E15" t="s">
@@ -6033,7 +6038,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="90" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6043,7 +6048,7 @@
       <c r="C16" t="s">
         <v>305</v>
       </c>
-      <c r="D16" s="126">
+      <c r="D16" s="112">
         <v>2</v>
       </c>
       <c r="E16" t="s">
@@ -6058,11 +6063,8 @@
       <c r="I16" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="J16" s="91" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6072,7 +6074,7 @@
       <c r="C17" t="s">
         <v>306</v>
       </c>
-      <c r="D17" s="126">
+      <c r="D17" s="112">
         <v>2</v>
       </c>
       <c r="E17" t="s">
@@ -6086,9 +6088,6 @@
       </c>
       <c r="I17" s="32" t="s">
         <v>189</v>
-      </c>
-      <c r="J17" s="91" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.2">
@@ -6101,7 +6100,7 @@
       <c r="C18" s="107" t="s">
         <v>316</v>
       </c>
-      <c r="D18" s="127" t="s">
+      <c r="D18" s="113" t="s">
         <v>329</v>
       </c>
       <c r="E18" t="s">
@@ -6116,8 +6115,11 @@
       <c r="I18" s="32" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="J18" s="91" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>308</v>
       </c>
@@ -6127,7 +6129,7 @@
       <c r="C19" t="s">
         <v>315</v>
       </c>
-      <c r="D19" s="126">
+      <c r="D19" s="112">
         <v>2</v>
       </c>
       <c r="E19" t="s">
@@ -6141,6 +6143,9 @@
       </c>
       <c r="I19" s="32" t="s">
         <v>201</v>
+      </c>
+      <c r="J19" s="91" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.2">
@@ -6153,7 +6158,7 @@
       <c r="C20" t="s">
         <v>311</v>
       </c>
-      <c r="D20" s="126">
+      <c r="D20" s="112">
         <v>1</v>
       </c>
       <c r="E20" t="s">
@@ -6182,7 +6187,7 @@
       <c r="C21" t="s">
         <v>306</v>
       </c>
-      <c r="D21" s="126">
+      <c r="D21" s="112">
         <v>1</v>
       </c>
       <c r="E21" t="s">
@@ -6211,7 +6216,7 @@
       <c r="C22" t="s">
         <v>312</v>
       </c>
-      <c r="D22" s="126">
+      <c r="D22" s="112">
         <v>1</v>
       </c>
       <c r="E22" t="s">
@@ -6237,7 +6242,7 @@
       <c r="C23" t="s">
         <v>313</v>
       </c>
-      <c r="D23" s="126">
+      <c r="D23" s="112">
         <v>1</v>
       </c>
       <c r="E23" t="s">
@@ -6263,7 +6268,7 @@
       <c r="C24" t="s">
         <v>314</v>
       </c>
-      <c r="D24" s="126">
+      <c r="D24" s="112">
         <v>1</v>
       </c>
       <c r="E24" t="s">

</xml_diff>